<commit_message>
functional but all in main package, attempting to separate into custom packages
</commit_message>
<xml_diff>
--- a/Bourbon_Website_Data.xlsx
+++ b/Bourbon_Website_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t xml:space="preserve">Data to be Outsourced</t>
   </si>
@@ -43,16 +43,16 @@
     <t xml:space="preserve">Proof</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimated Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aroma Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flavor Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finish Notes</t>
+    <t xml:space="preserve">Estimated_Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aroma_Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flavor_Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish_Notes</t>
   </si>
   <si>
     <t xml:space="preserve">Mashbill</t>
@@ -61,10 +61,10 @@
     <t xml:space="preserve">Sourced</t>
   </si>
   <si>
-    <t xml:space="preserve">Sourced from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Release</t>
+    <t xml:space="preserve">Sourced_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Released</t>
   </si>
   <si>
     <t xml:space="preserve">1792 Small Batch</t>
@@ -79,12 +79,51 @@
     <t xml:space="preserve">Kentucky</t>
   </si>
   <si>
-    <t xml:space="preserve">unknown</t>
-  </si>
-  <si>
     <t xml:space="preserve">4-8 years</t>
   </si>
   <si>
+    <t xml:space="preserve">Rye spice, Vanilla, Oak, Caramel, Honey, Fruit, Chocolate, Ethanol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rye Spice, Peppercorn, Vanilla, Chocolate, Caramel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spice, Vanilla, Caramel, Dark Fruit, Oak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1792 Sweet Wheat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Cherry, Vanilla, Oak, Spice, Toast, Leather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanilla, Caramel, Dried Fruit, Wood, Toast, Leather, Walnut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leather, Oak, Grain, Spice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1792 Aged 12 Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanilla, Wood, Smoke, Caramel, Toffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oak, Vanilla, Cocoa, Fruit, Toffee, Walnut, Rye Spice</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Oak, Toffee, </t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -93,213 +132,14 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Rye spice, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Vanilla, Oak, Caramel, Honey, Fruit, Chocolate, Ethanol</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rye Spice, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Peppercorn, Vanilla, Chocolate, Caramel</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Spice, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Vanilla, Caramel, Dark Fruit, Oak</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1792 Sweet Wheat</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Black Cherry, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Vanilla, Oak, Spice, Toast, Leather</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Vanilla, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Caramel, Dried Fruit, Wood, Toast, Leather, Walnut</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Leather, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Oak, Grain, Spice</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">wheated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1792 Aged 12 Years</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Vanilla, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Wood, Smoke, Caramel, Toffee</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Oak, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Vanilla, Cocoa, Fruit, Toffee, Walnut, Rye Spice</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Oak, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Toffee, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
       <t xml:space="preserve">Nut</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">high rye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annually</t>
+    <t xml:space="preserve">Bi-Annually</t>
   </si>
   <si>
     <t xml:space="preserve">1792 High Rye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAS</t>
   </si>
   <si>
     <r>
@@ -317,6 +157,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Oak, Dark Sugar, Fruit, Nut</t>
     </r>
@@ -337,6 +178,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Caramel, Apple, Cinnamon, Black Pepper, Leather</t>
     </r>
@@ -357,12 +199,10 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Oak, Rye Spice, Cinnamon, Sweet Fruit</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">High Rye</t>
   </si>
 </sst>
 </file>
@@ -372,7 +212,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -407,17 +247,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -583,16 +412,16 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,20 +499,34 @@
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>23</v>
       </c>
     </row>
@@ -703,8 +546,12 @@
       <c r="E4" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
@@ -714,15 +561,22 @@
       <c r="J4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="K4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -736,29 +590,37 @@
       <c r="E5" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="H5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -769,24 +631,35 @@
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>36</v>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>94.3</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
       <c r="H6" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>